<commit_message>
kein 15:00 Update moeglich
DerStandard hat heute Mittag die Darstellungen geaendert. Leider werden bei den Bundeslaendern nun die derzeit Erkrankten und Genesenen zusammengerechnet. Die berichteten Zahlen sind also derzeit auch hier nicht mehr vertrauenswuerdig
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jansteinfeld/SynologyDrive/GIT/COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AC0924-ABB1-0848-A2CC-B7B033FF52A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FD60E9-6DB7-394F-B48F-78125870472D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="22360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -621,7 +621,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F160" sqref="F160"/>
+      <selection pane="bottomLeft" activeCell="J165" sqref="J165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5680,8 +5680,11 @@
       <c r="C171" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F171" s="1">
+        <v>2</v>
+      </c>
       <c r="G171" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J171" s="1">
         <v>2</v>
@@ -5714,10 +5717,10 @@
         <v>2</v>
       </c>
       <c r="F172" s="1">
+        <v>13</v>
+      </c>
+      <c r="G172" s="1">
         <v>4</v>
-      </c>
-      <c r="G172" s="1">
-        <v>13</v>
       </c>
       <c r="H172" s="1">
         <v>4</v>
@@ -5924,10 +5927,12 @@
       <c r="J178" s="5"/>
       <c r="K178" s="5"/>
       <c r="L178" s="5"/>
-      <c r="M178" s="5"/>
+      <c r="M178" s="5">
+        <v>7971</v>
+      </c>
       <c r="N178" s="2" t="str">
         <f t="shared" ref="N178:N180" si="43">IF(SUM(D178:L178)=M178,"gleich","ungleich")</f>
-        <v>gleich</v>
+        <v>ungleich</v>
       </c>
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.2">
@@ -5940,10 +5945,12 @@
       <c r="C179" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M179" s="13"/>
+      <c r="M179" s="13">
+        <v>479</v>
+      </c>
       <c r="N179" s="2" t="str">
         <f t="shared" si="43"/>
-        <v>gleich</v>
+        <v>ungleich</v>
       </c>
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.2">
@@ -5956,10 +5963,12 @@
       <c r="C180" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M180" s="8"/>
+      <c r="M180" s="8">
+        <v>86</v>
+      </c>
       <c r="N180" s="2" t="str">
         <f t="shared" si="43"/>
-        <v>gleich</v>
+        <v>ungleich</v>
       </c>
     </row>
     <row r="181" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update 18:00 Zahlen weiterhin wenig vertrauenswuerdig
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10307"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Documents\Eigene_DATEN\private_Projekte\COVID-19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jansteinfeld/SynologyDrive/GIT/COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9CB27D-A3F0-E34E-AD26-DEE5D0EEF007}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="465" windowWidth="19200" windowHeight="22365"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="22360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$N$173</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,7 +214,35 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -643,23 +672,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N189"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L185" sqref="L185"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G162" sqref="G162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="13" width="5.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="2"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="3" width="11.5" style="1"/>
+    <col min="4" max="13" width="5.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5" style="2"/>
+    <col min="15" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>43886</v>
       </c>
@@ -732,7 +761,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>43886</v>
       </c>
@@ -750,7 +779,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>43886</v>
       </c>
@@ -768,7 +797,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>43886</v>
       </c>
@@ -791,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>43887</v>
       </c>
@@ -820,7 +849,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>43887</v>
       </c>
@@ -838,7 +867,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>43887</v>
       </c>
@@ -856,7 +885,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>43887</v>
       </c>
@@ -879,7 +908,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>43888</v>
       </c>
@@ -910,7 +939,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>43888</v>
       </c>
@@ -928,7 +957,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>43888</v>
       </c>
@@ -946,7 +975,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>43888</v>
       </c>
@@ -969,7 +998,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>43889</v>
       </c>
@@ -1000,7 +1029,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>43889</v>
       </c>
@@ -1018,7 +1047,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>43889</v>
       </c>
@@ -1036,7 +1065,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>43889</v>
       </c>
@@ -1059,7 +1088,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>43890</v>
       </c>
@@ -1109,7 +1138,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>43890</v>
       </c>
@@ -1127,7 +1156,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>43890</v>
       </c>
@@ -1145,7 +1174,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>43890</v>
       </c>
@@ -1168,7 +1197,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>43891</v>
       </c>
@@ -1219,7 +1248,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>43891</v>
       </c>
@@ -1237,7 +1266,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>43891</v>
       </c>
@@ -1255,7 +1284,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>43891</v>
       </c>
@@ -1278,7 +1307,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>43892</v>
       </c>
@@ -1327,7 +1356,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>43892</v>
       </c>
@@ -1345,7 +1374,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>43892</v>
       </c>
@@ -1363,7 +1392,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
         <v>43892</v>
       </c>
@@ -1386,7 +1415,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>43893</v>
       </c>
@@ -1431,7 +1460,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>43893</v>
       </c>
@@ -1449,7 +1478,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>43893</v>
       </c>
@@ -1467,7 +1496,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>43893</v>
       </c>
@@ -1490,7 +1519,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>43894</v>
       </c>
@@ -1537,7 +1566,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>43894</v>
       </c>
@@ -1558,7 +1587,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>43894</v>
       </c>
@@ -1576,7 +1605,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <v>43894</v>
       </c>
@@ -1599,7 +1628,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>43895</v>
       </c>
@@ -1644,7 +1673,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>43895</v>
       </c>
@@ -1665,7 +1694,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>43895</v>
       </c>
@@ -1683,7 +1712,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <v>43895</v>
       </c>
@@ -1706,7 +1735,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>43896</v>
       </c>
@@ -1751,7 +1780,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>43896</v>
       </c>
@@ -1772,7 +1801,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>43896</v>
       </c>
@@ -1790,7 +1819,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="9">
         <v>43896</v>
       </c>
@@ -1813,7 +1842,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>43897</v>
       </c>
@@ -1858,7 +1887,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>43897</v>
       </c>
@@ -1879,7 +1908,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>43897</v>
       </c>
@@ -1897,7 +1926,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
         <v>43897</v>
       </c>
@@ -1920,7 +1949,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>43898</v>
       </c>
@@ -1965,7 +1994,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>43898</v>
       </c>
@@ -1986,7 +2015,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>43898</v>
       </c>
@@ -2004,7 +2033,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="9">
         <v>43898</v>
       </c>
@@ -2027,7 +2056,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>43899</v>
       </c>
@@ -2072,7 +2101,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>43899</v>
       </c>
@@ -2093,7 +2122,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>43899</v>
       </c>
@@ -2111,7 +2140,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
         <v>43899</v>
       </c>
@@ -2134,7 +2163,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>43900</v>
       </c>
@@ -2179,7 +2208,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>43900</v>
       </c>
@@ -2203,7 +2232,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>43900</v>
       </c>
@@ -2221,7 +2250,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="9">
         <v>43900</v>
       </c>
@@ -2244,7 +2273,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>43901</v>
       </c>
@@ -2289,7 +2318,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>43901</v>
       </c>
@@ -2313,7 +2342,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>43901</v>
       </c>
@@ -2331,7 +2360,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="9">
         <v>43901</v>
       </c>
@@ -2354,7 +2383,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>43902</v>
       </c>
@@ -2399,7 +2428,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
         <v>43902</v>
       </c>
@@ -2423,7 +2452,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>43902</v>
       </c>
@@ -2444,7 +2473,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="9">
         <v>43902</v>
       </c>
@@ -2467,7 +2496,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>43903</v>
       </c>
@@ -2512,7 +2541,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>43903</v>
       </c>
@@ -2539,7 +2568,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>43903</v>
       </c>
@@ -2560,7 +2589,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="9">
         <v>43903</v>
       </c>
@@ -2583,7 +2612,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>43904</v>
       </c>
@@ -2628,7 +2657,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
         <v>43904</v>
       </c>
@@ -2655,7 +2684,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>43904</v>
       </c>
@@ -2676,7 +2705,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="9">
         <v>43904</v>
       </c>
@@ -2699,7 +2728,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>43905</v>
       </c>
@@ -2744,7 +2773,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="6">
         <v>43905</v>
       </c>
@@ -2771,7 +2800,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="6">
         <v>43905</v>
       </c>
@@ -2792,7 +2821,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="9">
         <v>43905</v>
       </c>
@@ -2815,7 +2844,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>43906</v>
       </c>
@@ -2860,7 +2889,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="6">
         <v>43906</v>
       </c>
@@ -2887,7 +2916,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="6">
         <v>43906</v>
       </c>
@@ -2911,7 +2940,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="9">
         <v>43906</v>
       </c>
@@ -2934,7 +2963,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>43907</v>
       </c>
@@ -2979,7 +3008,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
         <v>43907</v>
       </c>
@@ -3006,7 +3035,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
         <v>43907</v>
       </c>
@@ -3030,7 +3059,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="9">
         <v>43907</v>
       </c>
@@ -3053,7 +3082,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>43908</v>
       </c>
@@ -3098,7 +3127,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
         <v>43908</v>
       </c>
@@ -3125,7 +3154,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
         <v>43908</v>
       </c>
@@ -3149,7 +3178,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="9">
         <v>43908</v>
       </c>
@@ -3172,7 +3201,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>43909</v>
       </c>
@@ -3217,7 +3246,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
         <v>43909</v>
       </c>
@@ -3244,7 +3273,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
         <v>43909</v>
       </c>
@@ -3268,7 +3297,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="9">
         <v>43909</v>
       </c>
@@ -3291,7 +3320,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>43909</v>
       </c>
@@ -3336,7 +3365,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="6">
         <v>43909</v>
       </c>
@@ -3363,7 +3392,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="6">
         <v>43909</v>
       </c>
@@ -3390,7 +3419,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="9">
         <v>43909</v>
       </c>
@@ -3413,7 +3442,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>43910</v>
       </c>
@@ -3458,7 +3487,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="6">
         <v>43910</v>
       </c>
@@ -3485,7 +3514,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="6">
         <v>43910</v>
       </c>
@@ -3512,7 +3541,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="9">
         <v>43910</v>
       </c>
@@ -3535,7 +3564,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>43910</v>
       </c>
@@ -3580,7 +3609,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="6">
         <v>43910</v>
       </c>
@@ -3607,7 +3636,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="6">
         <v>43910</v>
       </c>
@@ -3634,7 +3663,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="9">
         <v>43910</v>
       </c>
@@ -3657,7 +3686,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>43911</v>
       </c>
@@ -3702,7 +3731,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="6">
         <v>43911</v>
       </c>
@@ -3729,7 +3758,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="6">
         <v>43911</v>
       </c>
@@ -3756,7 +3785,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="9">
         <v>43911</v>
       </c>
@@ -3779,7 +3808,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>43911</v>
       </c>
@@ -3824,7 +3853,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="6">
         <v>43911</v>
       </c>
@@ -3851,7 +3880,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="6">
         <v>43911</v>
       </c>
@@ -3878,7 +3907,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="9">
         <v>43911</v>
       </c>
@@ -3901,7 +3930,7 @@
         <v>2932</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>43912</v>
       </c>
@@ -3946,7 +3975,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="6">
         <v>43912</v>
       </c>
@@ -3973,7 +4002,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="6">
         <v>43912</v>
       </c>
@@ -4003,7 +4032,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="9">
         <v>43912</v>
       </c>
@@ -4026,7 +4055,7 @@
         <v>2823</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="3">
         <v>43912</v>
       </c>
@@ -4071,7 +4100,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="6">
         <v>43912</v>
       </c>
@@ -4098,7 +4127,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="6">
         <v>43912</v>
       </c>
@@ -4134,7 +4163,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="9">
         <v>43912</v>
       </c>
@@ -4157,7 +4186,7 @@
         <v>2823</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="3">
         <v>43913</v>
       </c>
@@ -4202,7 +4231,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="6">
         <v>43913</v>
       </c>
@@ -4229,7 +4258,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
         <v>43913</v>
       </c>
@@ -4265,7 +4294,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="9">
         <v>43913</v>
       </c>
@@ -4288,7 +4317,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>43913</v>
       </c>
@@ -4333,7 +4362,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" s="6">
         <v>43913</v>
       </c>
@@ -4360,7 +4389,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="6">
         <v>43913</v>
       </c>
@@ -4399,7 +4428,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" s="9">
         <v>43913</v>
       </c>
@@ -4422,7 +4451,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>43914</v>
       </c>
@@ -4467,7 +4496,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" s="6">
         <v>43914</v>
       </c>
@@ -4494,7 +4523,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" s="6">
         <v>43914</v>
       </c>
@@ -4533,7 +4562,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" s="9">
         <v>43914</v>
       </c>
@@ -4556,7 +4585,7 @@
         <v>4962</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" s="3">
         <v>43914</v>
       </c>
@@ -4601,7 +4630,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" s="6">
         <v>43914</v>
       </c>
@@ -4628,7 +4657,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" s="6">
         <v>43914</v>
       </c>
@@ -4667,7 +4696,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" s="9">
         <v>43914</v>
       </c>
@@ -4690,7 +4719,7 @@
         <v>4962</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" s="3">
         <v>43915</v>
       </c>
@@ -4735,7 +4764,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" s="6">
         <v>43915</v>
       </c>
@@ -4762,7 +4791,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" s="6">
         <v>43915</v>
       </c>
@@ -4801,7 +4830,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" s="9">
         <v>43915</v>
       </c>
@@ -4824,7 +4853,7 @@
         <v>4016</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
         <v>43915</v>
       </c>
@@ -4869,7 +4898,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" s="6">
         <v>43915</v>
       </c>
@@ -4896,7 +4925,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" s="6">
         <v>43915</v>
       </c>
@@ -4935,7 +4964,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" s="9">
         <v>43915</v>
       </c>
@@ -4958,7 +4987,7 @@
         <v>4016</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" s="3">
         <v>43916</v>
       </c>
@@ -5003,7 +5032,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" s="6">
         <v>43916</v>
       </c>
@@ -5030,7 +5059,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" s="6">
         <v>43916</v>
       </c>
@@ -5072,7 +5101,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" s="9">
         <v>43916</v>
       </c>
@@ -5095,7 +5124,7 @@
         <v>3588</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>43916</v>
       </c>
@@ -5140,7 +5169,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" s="6">
         <v>43916</v>
       </c>
@@ -5167,7 +5196,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" s="6">
         <v>43916</v>
       </c>
@@ -5209,7 +5238,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" s="9">
         <v>43916</v>
       </c>
@@ -5232,7 +5261,7 @@
         <v>3588</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" s="3">
         <v>43917</v>
       </c>
@@ -5277,7 +5306,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" s="6">
         <v>43917</v>
       </c>
@@ -5304,7 +5333,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" s="6">
         <v>43917</v>
       </c>
@@ -5349,7 +5378,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161" s="6">
         <v>43917</v>
       </c>
@@ -5372,7 +5401,7 @@
         <v>3557</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162" s="3">
         <v>43917</v>
       </c>
@@ -5417,7 +5446,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163" s="6">
         <v>43917</v>
       </c>
@@ -5444,7 +5473,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164" s="6">
         <v>43917</v>
       </c>
@@ -5489,7 +5518,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165" s="6">
         <v>43917</v>
       </c>
@@ -5512,7 +5541,7 @@
         <v>3557</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166" s="3">
         <v>43918</v>
       </c>
@@ -5557,7 +5586,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A167" s="6">
         <v>43918</v>
       </c>
@@ -5584,7 +5613,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168" s="6">
         <v>43918</v>
       </c>
@@ -5629,7 +5658,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A169" s="6">
         <v>43918</v>
       </c>
@@ -5652,7 +5681,7 @@
         <v>3299</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
         <v>43918</v>
       </c>
@@ -5697,7 +5726,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171" s="6">
         <v>43918</v>
       </c>
@@ -5727,7 +5756,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A172" s="6">
         <v>43918</v>
       </c>
@@ -5772,7 +5801,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A173" s="6">
         <v>43918</v>
       </c>
@@ -5795,7 +5824,7 @@
         <v>3299</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A174" s="3">
         <v>43919</v>
       </c>
@@ -5806,31 +5835,31 @@
         <v>13</v>
       </c>
       <c r="D174" s="5">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E174" s="5">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F174" s="5">
-        <v>1257</v>
+        <v>1214</v>
       </c>
       <c r="G174" s="5">
-        <v>1395</v>
+        <v>1331</v>
       </c>
       <c r="H174" s="5">
-        <v>789</v>
+        <v>755</v>
       </c>
       <c r="I174" s="5">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J174" s="5">
-        <v>1897</v>
+        <v>1671</v>
       </c>
       <c r="K174" s="5">
-        <v>576</v>
+        <v>564</v>
       </c>
       <c r="L174" s="5">
-        <v>1066</v>
+        <v>1055</v>
       </c>
       <c r="M174" s="5">
         <v>7726</v>
@@ -5840,7 +5869,7 @@
         <v>ungleich</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A175" s="6">
         <v>43919</v>
       </c>
@@ -5849,6 +5878,33 @@
       </c>
       <c r="C175" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="D175" s="1">
+        <v>4</v>
+      </c>
+      <c r="E175" s="1">
+        <v>8</v>
+      </c>
+      <c r="F175" s="1">
+        <v>43</v>
+      </c>
+      <c r="G175" s="1">
+        <v>64</v>
+      </c>
+      <c r="H175" s="1">
+        <v>34</v>
+      </c>
+      <c r="I175" s="1">
+        <v>1</v>
+      </c>
+      <c r="J175" s="1">
+        <v>226</v>
+      </c>
+      <c r="K175" s="1">
+        <v>12</v>
+      </c>
+      <c r="L175" s="1">
+        <v>11</v>
       </c>
       <c r="M175" s="13">
         <v>479</v>
@@ -5858,7 +5914,7 @@
         <v>ungleich</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176" s="6">
         <v>43919</v>
       </c>
@@ -5903,7 +5959,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177" s="6">
         <v>43919</v>
       </c>
@@ -5922,9 +5978,11 @@
       <c r="J177" s="11"/>
       <c r="K177" s="11"/>
       <c r="L177" s="11"/>
-      <c r="M177" s="12"/>
-    </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M177" s="12">
+        <v>3691</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A178" s="3">
         <v>43919</v>
       </c>
@@ -5935,31 +5993,31 @@
         <v>13</v>
       </c>
       <c r="D178" s="5">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E178" s="5">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="F178" s="5">
-        <v>1331</v>
+        <v>1288</v>
       </c>
       <c r="G178" s="5">
-        <v>1444</v>
+        <v>1380</v>
       </c>
       <c r="H178" s="5">
-        <v>794</v>
+        <v>760</v>
       </c>
       <c r="I178" s="5">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J178" s="5">
-        <v>1934</v>
+        <v>1708</v>
       </c>
       <c r="K178" s="5">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="L178" s="5">
-        <v>1080</v>
+        <v>1069</v>
       </c>
       <c r="M178" s="5">
         <v>791</v>
@@ -5969,7 +6027,7 @@
         <v>ungleich</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A179" s="6">
         <v>43919</v>
       </c>
@@ -5978,6 +6036,33 @@
       </c>
       <c r="C179" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="D179" s="1">
+        <v>4</v>
+      </c>
+      <c r="E179" s="1">
+        <v>8</v>
+      </c>
+      <c r="F179" s="1">
+        <v>43</v>
+      </c>
+      <c r="G179" s="1">
+        <v>64</v>
+      </c>
+      <c r="H179" s="1">
+        <v>34</v>
+      </c>
+      <c r="I179" s="1">
+        <v>1</v>
+      </c>
+      <c r="J179" s="1">
+        <v>226</v>
+      </c>
+      <c r="K179" s="1">
+        <v>12</v>
+      </c>
+      <c r="L179" s="1">
+        <v>11</v>
       </c>
       <c r="M179" s="13">
         <v>479</v>
@@ -5987,7 +6072,7 @@
         <v>ungleich</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A180" s="6">
         <v>43919</v>
       </c>
@@ -6032,7 +6117,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A181" s="6">
         <v>43919</v>
       </c>
@@ -6051,9 +6136,11 @@
       <c r="J181" s="11"/>
       <c r="K181" s="11"/>
       <c r="L181" s="11"/>
-      <c r="M181" s="12"/>
-    </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M181" s="12">
+        <v>3691</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182" s="3">
         <v>43920</v>
       </c>
@@ -6064,41 +6151,41 @@
         <v>13</v>
       </c>
       <c r="D182" s="5">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E182" s="5">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="F182" s="5">
-        <v>1367</v>
+        <v>1281</v>
       </c>
       <c r="G182" s="5">
-        <v>1502</v>
+        <v>1401</v>
       </c>
       <c r="H182" s="5">
-        <v>845</v>
+        <v>811</v>
       </c>
       <c r="I182" s="5">
-        <v>910</v>
+        <v>882</v>
       </c>
       <c r="J182" s="5">
-        <v>1991</v>
+        <v>1721</v>
       </c>
       <c r="K182" s="5">
-        <v>605</v>
+        <v>558</v>
       </c>
       <c r="L182" s="5">
-        <v>1095</v>
+        <v>1084</v>
       </c>
       <c r="M182" s="5">
-        <v>8393</v>
+        <v>8248</v>
       </c>
       <c r="N182" s="2" t="str">
         <f t="shared" ref="N182:N184" si="44">IF(SUM(D182:L182)=M182,"gleich","ungleich")</f>
         <v>ungleich</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183" s="6">
         <v>43920</v>
       </c>
@@ -6107,6 +6194,33 @@
       </c>
       <c r="C183" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="D183" s="1">
+        <v>4</v>
+      </c>
+      <c r="E183" s="1">
+        <v>13</v>
+      </c>
+      <c r="F183" s="1">
+        <v>86</v>
+      </c>
+      <c r="G183" s="1">
+        <v>101</v>
+      </c>
+      <c r="H183" s="1">
+        <v>34</v>
+      </c>
+      <c r="I183" s="1">
+        <v>28</v>
+      </c>
+      <c r="J183" s="1">
+        <v>270</v>
+      </c>
+      <c r="K183" s="1">
+        <v>47</v>
+      </c>
+      <c r="L183" s="1">
+        <v>11</v>
       </c>
       <c r="M183" s="13">
         <v>479</v>
@@ -6116,7 +6230,7 @@
         <v>ungleich</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A184" s="6">
         <v>43920</v>
       </c>
@@ -6161,7 +6275,7 @@
         <v>gleich</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185" s="6">
         <v>43920</v>
       </c>
@@ -6180,9 +6294,11 @@
       <c r="J185" s="11"/>
       <c r="K185" s="11"/>
       <c r="L185" s="11"/>
-      <c r="M185" s="12"/>
-    </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M185" s="12">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186" s="3">
         <v>43920</v>
       </c>
@@ -6192,22 +6308,42 @@
       <c r="C186" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D186" s="5"/>
-      <c r="E186" s="5"/>
-      <c r="F186" s="5"/>
-      <c r="G186" s="5"/>
-      <c r="H186" s="5"/>
-      <c r="I186" s="5"/>
-      <c r="J186" s="5"/>
-      <c r="K186" s="5"/>
-      <c r="L186" s="5"/>
-      <c r="M186" s="5"/>
+      <c r="D186" s="5">
+        <v>166</v>
+      </c>
+      <c r="E186" s="5">
+        <v>246</v>
+      </c>
+      <c r="F186" s="5">
+        <v>1419</v>
+      </c>
+      <c r="G186" s="5">
+        <v>1427</v>
+      </c>
+      <c r="H186" s="5">
+        <v>805</v>
+      </c>
+      <c r="I186" s="5">
+        <v>906</v>
+      </c>
+      <c r="J186" s="5">
+        <v>1922</v>
+      </c>
+      <c r="K186" s="5">
+        <v>568</v>
+      </c>
+      <c r="L186" s="5">
+        <v>1174</v>
+      </c>
+      <c r="M186" s="5">
+        <v>8633</v>
+      </c>
       <c r="N186" s="2" t="str">
-        <f t="shared" ref="N186:N188" si="45">IF(SUM(D186:L186)=M186,"gleich","ungleich")</f>
-        <v>gleich</v>
-      </c>
-    </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N186:N189" si="45">IF(SUM(D186:L186)=M186,"gleich","ungleich")</f>
+        <v>gleich</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187" s="6">
         <v>43920</v>
       </c>
@@ -6217,13 +6353,42 @@
       <c r="C187" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M187" s="13"/>
+      <c r="D187" s="1">
+        <v>10</v>
+      </c>
+      <c r="E187" s="1">
+        <v>13</v>
+      </c>
+      <c r="F187" s="1">
+        <v>86</v>
+      </c>
+      <c r="G187" s="1">
+        <v>101</v>
+      </c>
+      <c r="H187" s="1">
+        <v>43</v>
+      </c>
+      <c r="I187" s="1">
+        <v>28</v>
+      </c>
+      <c r="J187" s="1">
+        <v>270</v>
+      </c>
+      <c r="K187" s="1">
+        <v>47</v>
+      </c>
+      <c r="L187" s="1">
+        <v>38</v>
+      </c>
+      <c r="M187" s="13">
+        <v>636</v>
+      </c>
       <c r="N187" s="2" t="str">
         <f t="shared" si="45"/>
         <v>gleich</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188" s="6">
         <v>43920</v>
       </c>
@@ -6233,13 +6398,42 @@
       <c r="C188" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M188" s="8"/>
+      <c r="D188" s="1">
+        <v>3</v>
+      </c>
+      <c r="E188" s="1">
+        <v>2</v>
+      </c>
+      <c r="F188" s="1">
+        <v>28</v>
+      </c>
+      <c r="G188" s="1">
+        <v>7</v>
+      </c>
+      <c r="H188" s="1">
+        <v>7</v>
+      </c>
+      <c r="I188" s="1">
+        <v>24</v>
+      </c>
+      <c r="J188" s="1">
+        <v>13</v>
+      </c>
+      <c r="K188" s="1">
+        <v>1</v>
+      </c>
+      <c r="L188" s="1">
+        <v>23</v>
+      </c>
+      <c r="M188" s="8">
+        <v>108</v>
+      </c>
       <c r="N188" s="2" t="str">
         <f t="shared" si="45"/>
         <v>gleich</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A189" s="6">
         <v>43920</v>
       </c>
@@ -6258,11 +6452,357 @@
       <c r="J189" s="11"/>
       <c r="K189" s="11"/>
       <c r="L189" s="11"/>
-      <c r="M189" s="12"/>
+      <c r="M189" s="12">
+        <v>3014</v>
+      </c>
+      <c r="N189" s="2" t="str">
+        <f t="shared" si="45"/>
+        <v>ungleich</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A190" s="3">
+        <v>43921</v>
+      </c>
+      <c r="B190" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D190" s="5">
+        <v>168</v>
+      </c>
+      <c r="E190" s="5">
+        <v>252</v>
+      </c>
+      <c r="F190" s="5">
+        <v>1437</v>
+      </c>
+      <c r="G190" s="5">
+        <v>1455</v>
+      </c>
+      <c r="H190" s="5">
+        <v>859</v>
+      </c>
+      <c r="I190" s="5">
+        <v>948</v>
+      </c>
+      <c r="J190" s="5">
+        <v>1951</v>
+      </c>
+      <c r="K190" s="5">
+        <v>578</v>
+      </c>
+      <c r="L190" s="5">
+        <v>1242</v>
+      </c>
+      <c r="M190" s="5">
+        <v>8890</v>
+      </c>
+      <c r="N190" s="2" t="str">
+        <f t="shared" ref="N190:N193" si="46">IF(SUM(D190:L190)=M190,"gleich","ungleich")</f>
+        <v>gleich</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A191" s="6">
+        <v>43921</v>
+      </c>
+      <c r="B191" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D191" s="1">
+        <v>10</v>
+      </c>
+      <c r="E191" s="1">
+        <v>13</v>
+      </c>
+      <c r="F191" s="1">
+        <v>86</v>
+      </c>
+      <c r="G191" s="1">
+        <v>101</v>
+      </c>
+      <c r="H191" s="1">
+        <v>43</v>
+      </c>
+      <c r="I191" s="1">
+        <v>28</v>
+      </c>
+      <c r="J191" s="1">
+        <v>270</v>
+      </c>
+      <c r="K191" s="1">
+        <v>47</v>
+      </c>
+      <c r="L191" s="1">
+        <v>38</v>
+      </c>
+      <c r="M191" s="13">
+        <v>636</v>
+      </c>
+      <c r="N191" s="2" t="str">
+        <f t="shared" si="46"/>
+        <v>gleich</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A192" s="6">
+        <v>43921</v>
+      </c>
+      <c r="B192" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D192" s="1">
+        <v>3</v>
+      </c>
+      <c r="E192" s="1">
+        <v>2</v>
+      </c>
+      <c r="F192" s="1">
+        <v>28</v>
+      </c>
+      <c r="G192" s="1">
+        <v>7</v>
+      </c>
+      <c r="H192" s="1">
+        <v>7</v>
+      </c>
+      <c r="I192" s="1">
+        <v>24</v>
+      </c>
+      <c r="J192" s="1">
+        <v>13</v>
+      </c>
+      <c r="K192" s="1">
+        <v>1</v>
+      </c>
+      <c r="L192" s="1">
+        <v>23</v>
+      </c>
+      <c r="M192" s="8">
+        <v>108</v>
+      </c>
+      <c r="N192" s="2" t="str">
+        <f t="shared" si="46"/>
+        <v>gleich</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A193" s="6">
+        <v>43921</v>
+      </c>
+      <c r="B193" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C193" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D193" s="11"/>
+      <c r="E193" s="11"/>
+      <c r="F193" s="11"/>
+      <c r="G193" s="11"/>
+      <c r="H193" s="11"/>
+      <c r="I193" s="11"/>
+      <c r="J193" s="11"/>
+      <c r="K193" s="11"/>
+      <c r="L193" s="11"/>
+      <c r="M193" s="12">
+        <v>2889</v>
+      </c>
+      <c r="N193" s="2" t="str">
+        <f t="shared" si="46"/>
+        <v>ungleich</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A194" s="3">
+        <v>43921</v>
+      </c>
+      <c r="B194" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="C194" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D194" s="5">
+        <v>172</v>
+      </c>
+      <c r="E194" s="5">
+        <v>258</v>
+      </c>
+      <c r="F194" s="5">
+        <v>1519</v>
+      </c>
+      <c r="G194" s="5">
+        <v>1501</v>
+      </c>
+      <c r="H194" s="5">
+        <v>865</v>
+      </c>
+      <c r="I194" s="5">
+        <v>1002</v>
+      </c>
+      <c r="J194" s="5">
+        <v>2068</v>
+      </c>
+      <c r="K194" s="5">
+        <v>597</v>
+      </c>
+      <c r="L194" s="5">
+        <v>1342</v>
+      </c>
+      <c r="M194" s="5">
+        <v>8865</v>
+      </c>
+      <c r="N194" s="2" t="str">
+        <f t="shared" ref="N194:N197" si="47">IF(SUM(D194:L194)=M194,"gleich","ungleich")</f>
+        <v>ungleich</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A195" s="6">
+        <v>43921</v>
+      </c>
+      <c r="B195" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D195" s="1">
+        <v>10</v>
+      </c>
+      <c r="E195" s="1">
+        <v>13</v>
+      </c>
+      <c r="F195" s="1">
+        <v>86</v>
+      </c>
+      <c r="G195" s="1">
+        <v>101</v>
+      </c>
+      <c r="H195" s="1">
+        <v>43</v>
+      </c>
+      <c r="I195" s="1">
+        <v>28</v>
+      </c>
+      <c r="J195" s="1">
+        <v>270</v>
+      </c>
+      <c r="K195" s="1">
+        <v>47</v>
+      </c>
+      <c r="L195" s="1">
+        <v>38</v>
+      </c>
+      <c r="M195" s="13">
+        <v>1095</v>
+      </c>
+      <c r="N195" s="2" t="str">
+        <f t="shared" si="47"/>
+        <v>ungleich</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A196" s="6">
+        <v>43921</v>
+      </c>
+      <c r="B196" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D196" s="1">
+        <v>3</v>
+      </c>
+      <c r="E196" s="1">
+        <v>2</v>
+      </c>
+      <c r="F196" s="1">
+        <v>28</v>
+      </c>
+      <c r="G196" s="1">
+        <v>10</v>
+      </c>
+      <c r="H196" s="1">
+        <v>9</v>
+      </c>
+      <c r="I196" s="1">
+        <v>30</v>
+      </c>
+      <c r="J196" s="1">
+        <v>19</v>
+      </c>
+      <c r="K196" s="1">
+        <v>2</v>
+      </c>
+      <c r="L196" s="1">
+        <v>25</v>
+      </c>
+      <c r="M196" s="8">
+        <v>128</v>
+      </c>
+      <c r="N196" s="2" t="str">
+        <f t="shared" si="47"/>
+        <v>gleich</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A197" s="6">
+        <v>43921</v>
+      </c>
+      <c r="B197" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="C197" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D197" s="11"/>
+      <c r="E197" s="11"/>
+      <c r="F197" s="11"/>
+      <c r="G197" s="11"/>
+      <c r="H197" s="11"/>
+      <c r="I197" s="11"/>
+      <c r="J197" s="11"/>
+      <c r="K197" s="11"/>
+      <c r="L197" s="11"/>
+      <c r="M197" s="12">
+        <v>2889</v>
+      </c>
+      <c r="N197" s="2" t="str">
+        <f t="shared" si="47"/>
+        <v>ungleich</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N173"/>
-  <conditionalFormatting sqref="N1:N149 N190:N1048576">
+  <autoFilter ref="A1:N173" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="N1:N149 N198:N1048576">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+      <formula>"ungleich"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+      <formula>"gleich"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N150:N153">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+      <formula>"ungleich"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+      <formula>"gleich"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N154:N157">
     <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"ungleich"</formula>
     </cfRule>
@@ -6270,7 +6810,7 @@
       <formula>"gleich"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N150:N153">
+  <conditionalFormatting sqref="N158:N161">
     <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"ungleich"</formula>
     </cfRule>
@@ -6278,7 +6818,7 @@
       <formula>"gleich"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N154:N157">
+  <conditionalFormatting sqref="N162:N165">
     <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"ungleich"</formula>
     </cfRule>
@@ -6286,7 +6826,7 @@
       <formula>"gleich"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N158:N161">
+  <conditionalFormatting sqref="N166:N169">
     <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"ungleich"</formula>
     </cfRule>
@@ -6294,7 +6834,7 @@
       <formula>"gleich"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N162:N165">
+  <conditionalFormatting sqref="N170:N173">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"ungleich"</formula>
     </cfRule>
@@ -6302,7 +6842,7 @@
       <formula>"gleich"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N166:N169">
+  <conditionalFormatting sqref="N174:N177">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"ungleich"</formula>
     </cfRule>
@@ -6310,7 +6850,7 @@
       <formula>"gleich"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N170:N173">
+  <conditionalFormatting sqref="N178:N181">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"ungleich"</formula>
     </cfRule>
@@ -6318,7 +6858,7 @@
       <formula>"gleich"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N174:N177">
+  <conditionalFormatting sqref="N182:N185">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"ungleich"</formula>
     </cfRule>
@@ -6326,7 +6866,7 @@
       <formula>"gleich"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N178:N181">
+  <conditionalFormatting sqref="N186:N189">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"ungleich"</formula>
     </cfRule>
@@ -6334,7 +6874,7 @@
       <formula>"gleich"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N182:N185">
+  <conditionalFormatting sqref="N190:N193">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"ungleich"</formula>
     </cfRule>
@@ -6342,7 +6882,7 @@
       <formula>"gleich"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N186:N189">
+  <conditionalFormatting sqref="N194:N197">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"ungleich"</formula>
     </cfRule>

</xml_diff>